<commit_message>
Passage des instances de gouvernance de string en tag
</commit_message>
<xml_diff>
--- a/apps/backend/src/plans/plans/import-plan-aggregate/__fixtures__/nouveau-plan-valide.xlsx
+++ b/apps/backend/src/plans/plans/import-plan-aggregate/__fixtures__/nouveau-plan-valide.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="137">
   <si>
     <t>Présentation de l’action</t>
   </si>
@@ -227,6 +227,9 @@
   </si>
   <si>
     <t>Arranger la piste cyclable 2040-2044</t>
+  </si>
+  <si>
+    <t>Petite instance, blop</t>
   </si>
   <si>
     <r>
@@ -317,8 +320,7 @@
     <t>Ajouter caméra de surveillance au parking à vélo 2040-2044</t>
   </si>
   <si>
-    <t xml:space="preserve">Le CODIR est composé de 5 membres qui se reunissent 1 fois par trimestre.  
-Le COTECH est composé de 3 membres qui se réunissent 2 fois par an. </t>
+    <t>AAAA</t>
   </si>
   <si>
     <t>Ces informations devront être saisies directement sur la plateforme après l'import.</t>
@@ -610,7 +612,7 @@
     </font>
     <font>
       <sz val="12"/>
-      <color indexed="17"/>
+      <color indexed="13"/>
       <name val="Avenir Roman"/>
     </font>
     <font>
@@ -898,139 +900,139 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="5" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="6" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="7" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="7" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="8" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="7" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="7" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="7" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="59" fontId="8" fillId="7" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="8" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="7" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="11" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="8" fillId="5" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="8" fillId="5" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="10" fillId="5" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="60" fontId="8" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="60" fontId="8" fillId="5" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="60" fontId="8" fillId="7" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="60" fontId="8" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="8" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="59" fontId="8" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="8" fillId="5" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -1039,10 +1041,10 @@
     <xf numFmtId="49" fontId="12" fillId="9" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="7" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="13" fillId="3" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1066,11 +1068,11 @@
       <rgbColor rgb="ff5e88b1"/>
       <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ff808080"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="fffff2cc"/>
       <rgbColor rgb="ffdbe9f6"/>
       <rgbColor rgb="ffebc3b9"/>
       <rgbColor rgb="fff0f6fb"/>
-      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ff999999"/>
       <rgbColor rgb="fffff1f1"/>
       <rgbColor rgb="ffc00000"/>
@@ -1273,18 +1275,14 @@
     <a:spDef>
       <a:spPr>
         <a:solidFill>
-          <a:schemeClr val="accent6">
-            <a:hueOff val="-12436364"/>
-            <a:satOff val="-57894"/>
-            <a:lumOff val="3725"/>
-          </a:schemeClr>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1316,10 +1314,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1558,12 +1556,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1867,10 +1865,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -2416,47 +2414,49 @@
         <v>49</v>
       </c>
       <c r="E4" s="27"/>
-      <c r="F4" s="24"/>
+      <c r="F4" t="s" s="24">
+        <v>50</v>
+      </c>
       <c r="G4" s="24"/>
       <c r="H4" t="s" s="26">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I4" t="s" s="26">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J4" t="s" s="26">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K4" t="s" s="26">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="L4" t="s" s="26">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="M4" t="s" s="26">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="N4" t="s" s="26">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="O4" s="28"/>
       <c r="P4" t="s" s="24">
         <v>19</v>
       </c>
       <c r="Q4" t="s" s="26">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="R4" s="29">
         <v>3000</v>
       </c>
       <c r="S4" t="s" s="26">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="T4" s="30">
         <v>2000</v>
       </c>
       <c r="U4" t="s" s="26">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="V4" s="31">
         <v>999</v>
@@ -2465,72 +2465,72 @@
         <v>500</v>
       </c>
       <c r="X4" t="s" s="26">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="Y4" t="s" s="26">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="Z4" t="s" s="26">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AA4" t="s" s="26">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="AB4" t="s" s="26">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="AC4" t="s" s="24">
         <v>30</v>
       </c>
       <c r="AD4" t="s" s="26">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AE4" s="25"/>
       <c r="AF4" s="25"/>
       <c r="AG4" s="25"/>
       <c r="AH4" t="s" s="32">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="AI4" s="19"/>
     </row>
     <row r="5" ht="104.55" customHeight="1">
       <c r="A5" t="s" s="33">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B5" s="34"/>
       <c r="C5" s="35"/>
       <c r="D5" t="s" s="36">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E5" s="37"/>
       <c r="F5" t="s" s="33">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G5" s="33"/>
       <c r="H5" t="s" s="36">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I5" t="s" s="36">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="J5" t="s" s="36">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="K5" t="s" s="36">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="L5" t="s" s="36">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="M5" s="35"/>
       <c r="N5" t="s" s="36">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="O5" t="s" s="38">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="P5" t="s" s="33">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="Q5" s="35"/>
       <c r="R5" s="35"/>
@@ -2541,16 +2541,16 @@
       <c r="W5" s="35"/>
       <c r="X5" s="35"/>
       <c r="Y5" t="s" s="36">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="Z5" s="40"/>
       <c r="AA5" s="40"/>
       <c r="AB5" t="s" s="36">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AC5" s="33"/>
       <c r="AD5" t="s" s="36">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AE5" s="35"/>
       <c r="AF5" s="35"/>
@@ -2560,12 +2560,12 @@
     </row>
     <row r="6" ht="52.55" customHeight="1">
       <c r="A6" t="s" s="24">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B6" s="41"/>
       <c r="C6" s="25"/>
       <c r="D6" t="s" s="26">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E6" s="27"/>
       <c r="F6" s="24"/>
@@ -2574,21 +2574,21 @@
       <c r="I6" s="25"/>
       <c r="J6" s="25"/>
       <c r="K6" t="s" s="26">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="L6" t="s" s="26">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M6" t="s" s="26">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="N6" t="s" s="26">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="O6" s="28"/>
       <c r="P6" s="24"/>
       <c r="Q6" t="s" s="26">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="R6" s="29">
         <v>999</v>
@@ -2600,16 +2600,16 @@
       <c r="W6" s="25"/>
       <c r="X6" s="25"/>
       <c r="Y6" t="s" s="26">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="Z6" s="43"/>
       <c r="AA6" s="43"/>
       <c r="AB6" t="s" s="26">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AC6" s="24"/>
       <c r="AD6" t="s" s="26">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AE6" s="25"/>
       <c r="AF6" s="25"/>
@@ -2619,14 +2619,14 @@
     </row>
     <row r="7" ht="39.55" customHeight="1">
       <c r="A7" t="s" s="24">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B7" t="s" s="24">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C7" s="25"/>
       <c r="D7" t="s" s="26">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E7" s="27"/>
       <c r="F7" s="24"/>
@@ -2635,27 +2635,27 @@
       <c r="I7" s="25"/>
       <c r="J7" s="25"/>
       <c r="K7" t="s" s="26">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="L7" t="s" s="26">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="M7" t="s" s="26">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="N7" t="s" s="26">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="O7" s="28"/>
       <c r="P7" s="24"/>
       <c r="Q7" t="s" s="26">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="R7" s="29">
         <v>20000</v>
       </c>
       <c r="S7" t="s" s="26">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="T7" s="44">
         <v>2000</v>
@@ -2665,16 +2665,16 @@
       <c r="W7" s="25"/>
       <c r="X7" s="25"/>
       <c r="Y7" t="s" s="26">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="Z7" s="43"/>
       <c r="AA7" s="43"/>
       <c r="AB7" t="s" s="26">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AC7" s="24"/>
       <c r="AD7" t="s" s="26">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AE7" s="25"/>
       <c r="AF7" s="25"/>
@@ -2684,16 +2684,16 @@
     </row>
     <row r="8" ht="26.55" customHeight="1">
       <c r="A8" t="s" s="24">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B8" t="s" s="24">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C8" t="s" s="26">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D8" t="s" s="26">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E8" s="27"/>
       <c r="F8" s="24"/>
@@ -2729,19 +2729,19 @@
     </row>
     <row r="9" ht="78.55" customHeight="1">
       <c r="A9" t="s" s="33">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B9" t="s" s="33">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C9" t="s" s="36">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D9" t="s" s="36">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E9" t="s" s="33">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F9" s="33"/>
       <c r="G9" s="33"/>
@@ -2749,27 +2749,27 @@
       <c r="I9" s="35"/>
       <c r="J9" s="35"/>
       <c r="K9" t="s" s="36">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L9" t="s" s="36">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="M9" t="s" s="36">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="N9" t="s" s="36">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="O9" s="46"/>
       <c r="P9" s="33"/>
       <c r="Q9" t="s" s="36">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="R9" s="47">
         <v>10000</v>
       </c>
       <c r="S9" t="s" s="36">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="T9" s="48">
         <v>500</v>
@@ -2779,16 +2779,16 @@
       <c r="W9" s="35"/>
       <c r="X9" s="35"/>
       <c r="Y9" t="s" s="36">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="Z9" s="40"/>
       <c r="AA9" s="40"/>
       <c r="AB9" t="s" s="36">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AC9" s="33"/>
       <c r="AD9" t="s" s="36">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AE9" s="35"/>
       <c r="AF9" s="35"/>
@@ -2798,14 +2798,14 @@
     </row>
     <row r="10" ht="39.55" customHeight="1">
       <c r="A10" t="s" s="24">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B10" t="s" s="24">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C10" s="25"/>
       <c r="D10" t="s" s="26">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E10" s="27"/>
       <c r="F10" s="24"/>
@@ -2814,19 +2814,19 @@
       <c r="I10" s="25"/>
       <c r="J10" s="25"/>
       <c r="K10" t="s" s="26">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="L10" t="s" s="26">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="M10" t="s" s="26">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="N10" s="25"/>
       <c r="O10" s="28"/>
       <c r="P10" s="24"/>
       <c r="Q10" t="s" s="26">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="R10" s="29">
         <v>3000</v>
@@ -2841,11 +2841,11 @@
       <c r="Z10" s="43"/>
       <c r="AA10" s="43"/>
       <c r="AB10" t="s" s="26">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AC10" s="24"/>
       <c r="AD10" t="s" s="26">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AE10" s="25"/>
       <c r="AF10" s="25"/>
@@ -9788,7 +9788,7 @@
       <formula1>"Pas de participation citoyenne,Information,Consultation,Concertation,Co-construction"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB5:AB7 AB9:AB10">
-      <formula1>"VRAI,FAUX,FAUX"</formula1>
+      <formula1>"VRAI,FAUX,FAUX,FAUX"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB8 AB11:AB196">
       <formula1>"VRAI,FAUX"</formula1>
@@ -9823,10 +9823,10 @@
   <sheetData>
     <row r="1" ht="19.5" customHeight="1">
       <c r="A1" t="s" s="52">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B1" t="s" s="52">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C1" t="s" s="52">
         <v>25</v>
@@ -9835,135 +9835,135 @@
         <v>26</v>
       </c>
       <c r="E1" t="s" s="52">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" ht="19.5" customHeight="1">
       <c r="A2" t="s" s="53">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B2" t="s" s="53">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C2" t="s" s="53">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D2" t="s" s="53">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E2" t="s" s="53">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" ht="19.5" customHeight="1">
       <c r="A3" t="s" s="53">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B3" t="s" s="53">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C3" t="s" s="53">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D3" t="s" s="53">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E3" t="s" s="53">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" ht="19.5" customHeight="1">
       <c r="A4" t="s" s="53">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B4" t="s" s="53">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C4" t="s" s="53">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D4" t="s" s="53">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E4" t="s" s="53">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" ht="19.5" customHeight="1">
       <c r="A5" t="s" s="53">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B5" t="s" s="53">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C5" t="s" s="53">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D5" s="54"/>
       <c r="E5" t="s" s="53">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" ht="19.5" customHeight="1">
       <c r="A6" t="s" s="53">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B6" t="s" s="53">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C6" t="s" s="53">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D6" s="54"/>
       <c r="E6" t="s" s="53">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" ht="19.5" customHeight="1">
       <c r="A7" t="s" s="53">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B7" t="s" s="53">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C7" t="s" s="53">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D7" s="54"/>
       <c r="E7" s="54"/>
     </row>
     <row r="8" ht="19.5" customHeight="1">
       <c r="A8" t="s" s="53">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B8" t="s" s="53">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C8" t="s" s="53">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D8" s="54"/>
       <c r="E8" s="54"/>
     </row>
     <row r="9" ht="19.5" customHeight="1">
       <c r="A9" t="s" s="53">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B9" t="s" s="53">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C9" t="s" s="53">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D9" s="54"/>
       <c r="E9" s="54"/>
     </row>
     <row r="10" ht="19.5" customHeight="1">
       <c r="A10" t="s" s="53">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B10" t="s" s="53">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C10" s="54"/>
       <c r="D10" s="54"/>
@@ -9971,10 +9971,10 @@
     </row>
     <row r="11" ht="19.5" customHeight="1">
       <c r="A11" t="s" s="53">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B11" t="s" s="53">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C11" s="54"/>
       <c r="D11" s="54"/>
@@ -9982,10 +9982,10 @@
     </row>
     <row r="12" ht="19.5" customHeight="1">
       <c r="A12" t="s" s="53">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B12" t="s" s="53">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C12" s="54"/>
       <c r="D12" s="54"/>

</xml_diff>